<commit_message>
started table class, added present
</commit_message>
<xml_diff>
--- a/resources/test.xlsx
+++ b/resources/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amar\Git\sql_table_simple\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{950702EE-9DD0-4FA0-9163-CAE7F2666EF7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EA17B36-1BDB-4EEE-A008-728BDE13781F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{29EA5CD5-ECE9-4CF3-A867-536541DC2F12}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{4DAEF5F1-89FF-4019-8E61-393D8367E954}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -30,54 +30,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Vorname</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Kürzel</t>
-  </si>
-  <si>
-    <t>Budget</t>
-  </si>
-  <si>
-    <t>Hausnummer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max </t>
-  </si>
-  <si>
-    <t>Mustermann</t>
-  </si>
-  <si>
-    <t>MM</t>
-  </si>
-  <si>
-    <t>3c</t>
-  </si>
-  <si>
-    <t>Angela</t>
-  </si>
-  <si>
-    <t>Berkel</t>
-  </si>
-  <si>
-    <t>AB</t>
-  </si>
-  <si>
-    <t>Horst</t>
-  </si>
-  <si>
-    <t>Flamer</t>
-  </si>
-  <si>
-    <t>HF</t>
-  </si>
-  <si>
-    <t>20b</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+  <si>
+    <t>Kuerzel</t>
+  </si>
+  <si>
+    <t>Raum</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Uhrzeit</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>Di_10_12_Z6_HS4_SS_19</t>
+  </si>
+  <si>
+    <t>Z6_HS4</t>
+  </si>
+  <si>
+    <t>Di</t>
+  </si>
+  <si>
+    <t>10_12</t>
+  </si>
+  <si>
+    <t>SS_19</t>
+  </si>
+  <si>
+    <t>Do_8_10_Z6_HS4_SS_19</t>
+  </si>
+  <si>
+    <t>Do</t>
+  </si>
+  <si>
+    <t>8_10</t>
+  </si>
+  <si>
+    <t>Di_10_12_Z6_HS4_SS_18</t>
+  </si>
+  <si>
+    <t>SS_18</t>
+  </si>
+  <si>
+    <t>Do_8_10_Z6_HS4_SS_18</t>
+  </si>
+  <si>
+    <t>Mi_14_16_Z6_HS1_WS_19_20</t>
+  </si>
+  <si>
+    <t>Z6_HS1</t>
+  </si>
+  <si>
+    <t>Mi</t>
+  </si>
+  <si>
+    <t>14_16</t>
+  </si>
+  <si>
+    <t>WS_19_20</t>
+  </si>
+  <si>
+    <t>Mi_16_18_Z6_HS1_WS_19_20</t>
+  </si>
+  <si>
+    <t>16_18</t>
+  </si>
+  <si>
+    <t>Mi_14_16_Z6_HS1_WS_18_19</t>
+  </si>
+  <si>
+    <t>WS_18_19</t>
+  </si>
+  <si>
+    <t>Mi_16_18_Z6_HS1_WS_18_19</t>
   </si>
 </sst>
 </file>
@@ -428,14 +458,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BE8B38-F610-4739-9130-47124F5AB0A5}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37371AAD-AF5C-4902-9618-14AEFC2FA6B3}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -464,45 +497,130 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
-        <v>50000</v>
+      <c r="D2" t="s">
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3">
-        <v>100000</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="D4">
-        <v>30000</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>